<commit_message>
Add Book backend view
</commit_message>
<xml_diff>
--- a/BookStore.xlsx
+++ b/BookStore.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7155" tabRatio="667" firstSheet="13" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="667" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="WebMaster" sheetId="13" r:id="rId1"/>
-    <sheet name="Merchant" sheetId="11" r:id="rId2"/>
-    <sheet name="Customer" sheetId="7" r:id="rId3"/>
+    <sheet name="Customer" sheetId="7" r:id="rId2"/>
+    <sheet name="Merchant" sheetId="11" r:id="rId3"/>
     <sheet name="Advertiser" sheetId="6" r:id="rId4"/>
     <sheet name="AdvertiseContract" sheetId="3" r:id="rId5"/>
     <sheet name="MerchantContract" sheetId="12" r:id="rId6"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="150">
   <si>
     <t>BookCategoryName</t>
   </si>
@@ -107,29 +107,6 @@
   </si>
   <si>
     <t>Robins Sharma</t>
-  </si>
-  <si>
-    <r>
-      <t>Bằng những lời chia sẻ thật ngắn gọn, dễ hiểu về những trải nghiệm và suy ngẫm trong đời, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF242424"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Robin Sharma </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF242424"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>tiếp tục phong cách viết của ông từ cuốn sách Điều vĩ đại đời thường để mang đến cho độc giả những bài viết như lời tâm sự, vừa chân thành vừa sâu sắc.</t>
-    </r>
   </si>
   <si>
     <t>Nếu tôi biết khi còn 20</t>
@@ -222,7 +199,7 @@
         <i/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -341,6 +318,21 @@
     <t>ContractLink</t>
   </si>
   <si>
+    <t>WEBMASTER</t>
+  </si>
+  <si>
+    <t>ACCOUNTANT</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>ADCENSOR</t>
+  </si>
+  <si>
+    <t>MERCHANTCENSOR</t>
+  </si>
+  <si>
     <t>Thảo</t>
   </si>
   <si>
@@ -443,58 +435,125 @@
     <t>Săn sách giá rẻ</t>
   </si>
   <si>
-    <t>kimlong.com.vn</t>
-  </si>
-  <si>
-    <t>viethung.com.vn</t>
-  </si>
-  <si>
-    <t>phongvu.com.vn</t>
-  </si>
-  <si>
-    <t>tiki.vn</t>
-  </si>
-  <si>
-    <t>WebMaster</t>
-  </si>
-  <si>
-    <t>Accountant</t>
-  </si>
-  <si>
-    <t>AdCensor</t>
-  </si>
-  <si>
-    <t>MerchantCensor</t>
-  </si>
-  <si>
-    <t>Admin</t>
+    <t>Athoner</t>
+  </si>
+  <si>
+    <t>Hai mươi sáu năm về trước có một học sinh hoàn thiện hoàn mĩ. Rất đẹp, rất giỏi, rất hòa đồng, ai cũng yêu quý, những lời tán tụng người ấy được truyền mãi qua các thế hệ học sinh của trường. Nhưng tên đầy đủ là gì, chết đi thế nào, thậm chí giới tính ra sao lại không một ai hay biết. Người ta chỉ rỉ tai nhau, bỗng nhiên giữa năm bạn ấy chết, trường lớp không sao thoát được nỗi buồn nhớ thương, họ bèn cư xử như thể học sinh này còn tồn tại. Bàn ghế để nguyên, bạn cùng lớp vẫn giả vờ nói chuyện với người đã khuất.</t>
+  </si>
+  <si>
+    <t>Yukito Ayatsuji</t>
+  </si>
+  <si>
+    <t>Nhà xuất bản văn học</t>
+  </si>
+  <si>
+    <t>Tokyo Hoàng Đạo Án</t>
+  </si>
+  <si>
+    <t>Soji Shimada</t>
+  </si>
+  <si>
+    <t>Hãy tới đây, hạ giới và vòm trời Bombô
+Ta sẽ giết các con và cháu ta
+Cắt thân thể chúng rời rã ra
+Ghép phần đẹp nhất thành người mới
+Mảnh miếng còn lại đem chôn xa
+Đối với phụ nữ, ta có niềm đam mê mãnh liệt. Đối với cái đẹp, ta nhất mực tôn sùng.
+Sau ba chục năm nghiên cứu chiêm tinh và giả kim thuật, ta ấp ủ ước vọng tạo ra một tấm thân phụ nữ toàn bích hơn hết thảy nhan sắc trên đời.
+Ta bí mật lên kế hoạch giết sáu đứa con gái và cháu gái trinh trắng trong nhà, lựa lấy đầu, ngực, bụng, hông, đùi và chân hoàn mỹ nhất để luyện thành một sinh thể mới. Những phần dư, ta sẽ đem chôn theo một sơ đồ hoàng đạo.</t>
+  </si>
+  <si>
+    <t>Kỹ Thuật Làm Bánh Ngọt - Cuốn Sách Cho Người Bắt Đầu Học Làm Bánh</t>
+  </si>
+  <si>
+    <t>Nhà Xuất Bản Phụ Nữ</t>
+  </si>
+  <si>
+    <t>Với một chiếc lò nướng bánh gia đình và một số dụng cụ, khi bạn làm đúng theo các bước hướng dẫn và công thức đảm bảo bạn luôn đi đúng đường, mùi thơm của bánh ngọt sẽ lan tỏa trong căn bếp nhà bạn.
+Cuốn Sách Cho Người Bắt Đầu Học Làm Bánh là những kiến thức cơ bản nhất mà một người bắt đầu làm quen với bột, lò nướng cần có: Gồm các kiến thức chung về nguyên liệu, dụng cụ làm bánh, các kỹ năng làm bánh cơ bản. Cuốn sách còn cung cấp các công thức làm bánh Cookies. Muffin, Cream Cake, Tart đơn giản, dễ làm nhưng cũng rất hấp dẫn, ngon miệng.</t>
+  </si>
+  <si>
+    <t>150 Thuật Ngữ Văn Học</t>
+  </si>
+  <si>
+    <t>Lại Nguyên Ân</t>
+  </si>
+  <si>
+    <t>Nhà Xuất Bản Văn Học</t>
+  </si>
+  <si>
+    <t>Truyện ngụ ngôn Êdốp</t>
+  </si>
+  <si>
+    <t>Nhà Xuất Bản Thời Đại</t>
+  </si>
+  <si>
+    <t>êdop</t>
+  </si>
+  <si>
+    <t>Truyện tranh thiếu nhi</t>
+  </si>
+  <si>
+    <t>Alixơ ở xứ sở diệu kỳ</t>
+  </si>
+  <si>
+    <t>Hàn Thuyên</t>
+  </si>
+  <si>
+    <t>Bằng những lời chia sẻ thật ngắn gọn, dễ hiểu về những trải nghiệm và suy ngẫm trong đời, Robin Sharma tiếp tục phong cách viết của ông từ cuốn sách Điều vĩ đại đời thường để mang đến cho độc giả những bài viết như lời tâm sự, vừa chân thành vừa sâu sắc.</t>
+  </si>
+  <si>
+    <r>
+      <t>150 Thuật Ngữ Văn Học</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF242424"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> - Với khoảng trên 150 mục từ THUẬT NGỮ VĂN HỌC, cuốnsách nhỏ này chưa thể bao quát toàn bộ các bình diện, cấp độ, sắc thái của một loại hiện tượng văn hoá nhân bản đặcsắc và vô cùng phong phú là văn học và các chuyên ngành nghiên cứu nó…</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF242424"/>
       <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -538,33 +597,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,19 +950,19 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.375" customWidth="1"/>
-    <col min="4" max="4" width="15.875" customWidth="1"/>
-    <col min="5" max="5" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -893,62 +971,62 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -965,7 +1043,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -977,7 +1055,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -988,68 +1066,68 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.25" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="18.25" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1065,46 +1143,46 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="14.25" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4">
         <v>1</v>
       </c>
@@ -1122,17 +1200,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1140,7 +1218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1148,7 +1226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1156,7 +1234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1171,267 +1249,511 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.75" customWidth="1"/>
-    <col min="3" max="3" width="17.75" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
-    <col min="5" max="5" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="26.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="15"/>
+    <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="4">
         <v>0</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="8">
         <v>45000</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="4">
         <v>20</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="4">
         <v>200</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="4">
         <v>14</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="4">
         <v>320</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="16">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
         <v>46000</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="4">
         <v>21</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="4">
         <v>150</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="4">
         <v>15</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="4">
         <v>239</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="M3" s="16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="90" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
+        <v>44000</v>
+      </c>
+      <c r="H4" s="4">
+        <v>22</v>
+      </c>
+      <c r="I4" s="4">
+        <v>155</v>
+      </c>
+      <c r="J4" s="4">
+        <v>13</v>
+      </c>
+      <c r="K4" s="4">
+        <v>252</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="16">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>55000</v>
+      </c>
+      <c r="H5" s="4">
+        <v>21</v>
+      </c>
+      <c r="I5" s="4">
+        <v>250</v>
+      </c>
+      <c r="J5" s="4">
+        <v>16</v>
+      </c>
+      <c r="K5" s="4">
+        <v>323</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>65000</v>
+      </c>
+      <c r="H6" s="8">
+        <v>25</v>
+      </c>
+      <c r="I6" s="8">
+        <v>270</v>
+      </c>
+      <c r="J6" s="8">
+        <v>13</v>
+      </c>
+      <c r="K6" s="13">
+        <v>234</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="16">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="270" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>45000</v>
+      </c>
+      <c r="H7" s="4">
+        <v>21</v>
+      </c>
+      <c r="I7" s="4">
+        <v>340</v>
+      </c>
+      <c r="J7" s="4">
+        <v>12</v>
+      </c>
+      <c r="K7" s="4">
+        <v>332</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="M7" s="16">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="8">
+        <v>54000</v>
+      </c>
+      <c r="H8" s="4">
+        <v>25</v>
+      </c>
+      <c r="I8" s="4">
+        <v>230</v>
+      </c>
+      <c r="J8" s="4">
+        <v>11</v>
+      </c>
+      <c r="K8" s="4">
+        <v>231</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="M8" s="16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>23000</v>
+      </c>
+      <c r="H9" s="4">
+        <v>32</v>
+      </c>
+      <c r="I9" s="4">
+        <v>354</v>
+      </c>
+      <c r="J9" s="4">
+        <v>21</v>
+      </c>
+      <c r="K9" s="4">
+        <v>332</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M9" s="15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>40000</v>
+      </c>
+      <c r="H10" s="4">
+        <v>7</v>
+      </c>
+      <c r="I10" s="4">
+        <v>643</v>
+      </c>
+      <c r="J10" s="4">
+        <v>23</v>
+      </c>
+      <c r="K10" s="6">
+        <v>588</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="M10" s="16">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1">
-        <v>4</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>44000</v>
-      </c>
-      <c r="H4" s="1">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1">
-        <v>155</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="E11" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8">
+        <v>23000</v>
+      </c>
+      <c r="H11" s="4">
         <v>13</v>
       </c>
-      <c r="K4" s="1">
-        <v>252</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4" s="2">
+      <c r="I11" s="4">
+        <v>231</v>
+      </c>
+      <c r="J11" s="4">
+        <v>21</v>
+      </c>
+      <c r="K11" s="4">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>55000</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="L11" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="M11" s="16">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H12" s="4">
         <v>21</v>
       </c>
-      <c r="I5" s="1">
-        <v>250</v>
-      </c>
-      <c r="J5" s="1">
-        <v>16</v>
-      </c>
-      <c r="K5" s="1">
-        <v>323</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="2">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2">
-        <v>65000</v>
-      </c>
-      <c r="H6" s="2">
-        <v>25</v>
-      </c>
-      <c r="I6" s="2">
-        <v>270</v>
-      </c>
-      <c r="J6" s="2">
-        <v>13</v>
-      </c>
-      <c r="K6" s="5">
-        <v>234</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="2">
-        <v>47</v>
+      <c r="I12" s="4">
+        <v>23</v>
+      </c>
+      <c r="K12" s="4">
+        <v>132</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="M12" s="16">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1448,55 +1770,55 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="17.75" customWidth="1"/>
-    <col min="5" max="5" width="53.375" customWidth="1"/>
-    <col min="6" max="6" width="20.625" customWidth="1"/>
-    <col min="8" max="8" width="19.875" customWidth="1"/>
-    <col min="9" max="9" width="13.375" customWidth="1"/>
-    <col min="10" max="10" width="13.125" customWidth="1"/>
-    <col min="11" max="11" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
         <v>63</v>
       </c>
-      <c r="K1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1504,10 +1826,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="G2">
         <v>200000</v>
@@ -1519,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1527,10 +1849,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="G3">
         <v>300000</v>
@@ -1542,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1550,10 +1872,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G4">
         <v>500000</v>
@@ -1575,35 +1897,35 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.75" customWidth="1"/>
-    <col min="3" max="3" width="13.875" customWidth="1"/>
-    <col min="4" max="4" width="14.25" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1614,7 +1936,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1625,7 +1947,7 @@
         <v>92000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1636,7 +1958,7 @@
         <v>88000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1647,7 +1969,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1671,36 +1993,36 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.875" customWidth="1"/>
-    <col min="7" max="7" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>75</v>
-      </c>
-      <c r="C1" t="s">
-        <v>76</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1710,14 +2032,14 @@
       <c r="C2">
         <v>50</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>45000</v>
       </c>
       <c r="E2">
         <v>2250000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1727,14 +2049,14 @@
       <c r="C3">
         <v>65</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>46000</v>
       </c>
       <c r="E3">
         <v>2990000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1744,14 +2066,14 @@
       <c r="C4">
         <v>34</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>44000</v>
       </c>
       <c r="E4">
         <v>1496000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1761,14 +2083,14 @@
       <c r="C5">
         <v>76</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>55000</v>
       </c>
       <c r="E5">
         <v>4180000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1778,7 +2100,7 @@
       <c r="C6">
         <v>45</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>65000</v>
       </c>
       <c r="E6">
@@ -1794,35 +2116,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1833,7 +2155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1844,7 +2166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1855,7 +2177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1866,7 +2188,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1884,204 +2206,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="22.125" customWidth="1"/>
-    <col min="6" max="6" width="31.75" customWidth="1"/>
-    <col min="7" max="7" width="29.75" customWidth="1"/>
-    <col min="8" max="8" width="19.375" customWidth="1"/>
-    <col min="9" max="9" width="16.75" customWidth="1"/>
-    <col min="11" max="11" width="16.25" customWidth="1"/>
-    <col min="12" max="12" width="18.875" customWidth="1"/>
-    <col min="13" max="13" width="23.625" customWidth="1"/>
-    <col min="14" max="14" width="15.125" customWidth="1"/>
-    <col min="16" max="16" width="12.125" customWidth="1"/>
-    <col min="17" max="17" width="23.875" customWidth="1"/>
-    <col min="18" max="18" width="18.75" customWidth="1"/>
-    <col min="19" max="19" width="8.875" customWidth="1"/>
-    <col min="21" max="21" width="13.25" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>48</v>
-      </c>
-      <c r="R1" t="s">
-        <v>49</v>
-      </c>
-      <c r="S1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>94</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C2">
-        <v>19001112</v>
-      </c>
-      <c r="D2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2">
-        <v>45342</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>102</v>
-      </c>
-      <c r="L2" t="s">
-        <v>94</v>
-      </c>
-      <c r="M2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N2">
-        <v>123123123</v>
-      </c>
-      <c r="O2" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" t="s">
-        <v>78</v>
-      </c>
-      <c r="S2">
         <v>0</v>
       </c>
-      <c r="T2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5">
         <v>0</v>
       </c>
-      <c r="U2" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3">
-        <v>12234332</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3">
-        <v>896895</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>101</v>
-      </c>
-      <c r="L3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" t="s">
-        <v>98</v>
-      </c>
-      <c r="N3">
-        <v>456432456</v>
-      </c>
-      <c r="O3" t="s">
-        <v>58</v>
-      </c>
-      <c r="P3" t="s">
-        <v>79</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2091,82 +2291,204 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.125" style="9"/>
-    <col min="4" max="4" width="12.75" customWidth="1"/>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="23.85546875" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" customWidth="1"/>
+    <col min="21" max="21" width="13.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="9" t="s">
-        <v>68</v>
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
       </c>
       <c r="C2">
+        <v>19001112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2">
+        <v>45342</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2">
+        <v>123123123</v>
+      </c>
+      <c r="O2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" t="s">
+        <v>77</v>
+      </c>
+      <c r="S2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
-        <v>69</v>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4">
+        <v>12234332</v>
+      </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3">
+        <v>896895</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5">
+      <c r="K3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" t="s">
+        <v>102</v>
+      </c>
+      <c r="M3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N3">
+        <v>456432456</v>
+      </c>
+      <c r="O3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" t="s">
+        <v>78</v>
+      </c>
+      <c r="S3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2179,79 +2501,76 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.375" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.25" customWidth="1"/>
-    <col min="6" max="6" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
       <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2267,54 +2586,54 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.25" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.25" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="16.125" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" t="s">
-        <v>88</v>
-      </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="F2" t="b">
         <v>1</v>
       </c>
@@ -2322,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2336,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2360,40 +2679,40 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="3" max="3" width="12.75" customWidth="1"/>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
-    <col min="5" max="5" width="14.25" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>2</v>
       </c>
@@ -2409,7 +2728,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2421,7 +2740,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2433,7 +2752,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>